<commit_message>
Completed Caddy X5RK | Challenger 100&500 Ongoing
</commit_message>
<xml_diff>
--- a/Cadillac/Status-Variables.xlsx
+++ b/Cadillac/Status-Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acfaa78c33d8f6c1/Desktop/CaddyTemp/CamaroCE/Cadillac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="428" documentId="13_ncr:40009_{048C9A78-2CE1-4D13-B54A-8D0626558D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D563E48-4745-41DD-B3D4-77BC12D0779F}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="13_ncr:40009_{048C9A78-2CE1-4D13-B54A-8D0626558D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184A95D7-C9B4-4750-B2F9-209F371A069E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="3" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="356">
   <si>
     <t>Vin</t>
   </si>
@@ -2497,7 +2497,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3255,7 +3255,7 @@
         <v>279</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>9</v>
@@ -3288,7 +3288,9 @@
       <c r="H21" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Completed N5RK | Challenger hitting unknown issue
</commit_message>
<xml_diff>
--- a/Cadillac/Status-Variables.xlsx
+++ b/Cadillac/Status-Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acfaa78c33d8f6c1/Desktop/CaddyTemp/CamaroCE/Cadillac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="430" documentId="13_ncr:40009_{048C9A78-2CE1-4D13-B54A-8D0626558D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184A95D7-C9B4-4750-B2F9-209F371A069E}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="13_ncr:40009_{048C9A78-2CE1-4D13-B54A-8D0626558D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08AEF5FF-9323-4C26-87D4-B636F113D093}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="3" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="356">
   <si>
     <t>Vin</t>
   </si>
@@ -2497,7 +2497,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3289,7 +3289,7 @@
         <v>276</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>9</v>
@@ -3322,7 +3322,9 @@
       <c r="H22" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>